<commit_message>
[UPDATE] - import done
</commit_message>
<xml_diff>
--- a/ListePersonnes.xlsx
+++ b/ListePersonnes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\assan\Documents\Projects\ProjetPsi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ProjetPsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41217D7-E96C-40D2-BBE8-51657DBAAB4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3475DFC-3395-478E-97F2-32E6E356DCF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A6D5398-05A1-9B40-A1C5-C6EB71C96023}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A6D5398-05A1-9B40-A1C5-C6EB71C96023}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="339">
   <si>
     <t>Ahmed</t>
   </si>
@@ -1027,13 +1027,34 @@
   </si>
   <si>
     <t>EMAIL</t>
+  </si>
+  <si>
+    <t>sakho</t>
+  </si>
+  <si>
+    <t>assane</t>
+  </si>
+  <si>
+    <t>NOM1</t>
+  </si>
+  <si>
+    <t>DS@dsdsd</t>
+  </si>
+  <si>
+    <t>ETU</t>
+  </si>
+  <si>
+    <t>APOGEE</t>
+  </si>
+  <si>
+    <t>STATUT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1043,6 +1064,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1065,14 +1094,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1385,27 +1417,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90909A8-F959-FB44-BCC9-568D79532649}">
-  <dimension ref="A1:E198"/>
+  <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.8984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.59765625" customWidth="1"/>
+    <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.625" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>50</v>
       </c>
@@ -1413,436 +1444,439 @@
         <v>330</v>
       </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>334</v>
+      </c>
+      <c r="B3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C3">
+        <v>78455</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="E3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>340001</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
+      <c r="C5">
         <v>340002</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
+      <c r="C6">
         <v>340003</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
+      <c r="C7">
         <v>340004</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
+      <c r="C8">
         <v>340005</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
+      <c r="C9">
         <v>340006</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
+      <c r="C10">
         <v>340007</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="E10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9">
+      <c r="C11">
         <v>340008</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="E11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10">
+      <c r="C12">
         <v>340009</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
+      <c r="C13">
         <v>340010</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="E13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
+      <c r="C14">
         <v>340011</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
+      <c r="C15">
         <v>340012</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
+      <c r="C16">
         <v>340013</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>27</v>
       </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
+      <c r="C17">
         <v>340014</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="E17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>29</v>
       </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
+      <c r="C18">
         <v>340015</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
+      <c r="C19">
         <v>340016</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="E19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>33</v>
       </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
+      <c r="C20">
         <v>340017</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>35</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19">
+      <c r="C21">
         <v>340018</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="E21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>37</v>
       </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
+      <c r="C22">
         <v>340019</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>39</v>
       </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-      <c r="D21">
+      <c r="C23">
         <v>340020</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>40</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22">
+      <c r="C24">
         <v>340021</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="E24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>42</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>43</v>
       </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-      <c r="D23">
+      <c r="C25">
         <v>340022</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="E25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>44</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>45</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
+      <c r="C26">
         <v>340023</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="E26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>47</v>
       </c>
-      <c r="C25">
-        <v>2</v>
-      </c>
-      <c r="D25">
+      <c r="C27">
         <v>340024</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="E27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>48</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>49</v>
       </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
+      <c r="C28">
         <v>340025</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>54</v>
       </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
+      <c r="C29">
         <v>340026</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="E29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>55</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>56</v>
       </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28">
+      <c r="C30">
         <v>340027</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="E30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>57</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>58</v>
       </c>
-      <c r="C29">
-        <v>2</v>
-      </c>
-      <c r="D29">
+      <c r="C31">
         <v>340028</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>340029</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31">
-        <v>340030</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1850,2338 +1884,2369 @@
         <v>60</v>
       </c>
       <c r="C32">
-        <v>2</v>
-      </c>
-      <c r="D32">
+        <v>340029</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33">
+        <v>340030</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34">
         <v>340031</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>63</v>
       </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33">
+      <c r="C35">
         <v>340032</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>62</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>63</v>
       </c>
-      <c r="C34">
-        <v>2</v>
-      </c>
-      <c r="D34">
+      <c r="C36">
         <v>340033</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>65</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>66</v>
       </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35">
+      <c r="C37">
         <v>340034</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="E37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>67</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-      <c r="D36">
+      <c r="C38">
         <v>340035</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="E38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>67</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>68</v>
       </c>
-      <c r="C37">
-        <v>2</v>
-      </c>
-      <c r="D37">
+      <c r="C39">
         <v>340036</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>69</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>70</v>
       </c>
-      <c r="C38">
-        <v>2</v>
-      </c>
-      <c r="D38">
+      <c r="C40">
         <v>340037</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="E40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>71</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>72</v>
       </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-      <c r="D39">
+      <c r="C41">
         <v>340038</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="E41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>73</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>74</v>
       </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-      <c r="D40">
+      <c r="C42">
         <v>340039</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="E42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>73</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>74</v>
       </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-      <c r="D41">
+      <c r="C43">
         <v>340040</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="E43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>75</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>76</v>
       </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-      <c r="D42">
+      <c r="C44">
         <v>340041</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="E44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>77</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B45" t="s">
         <v>72</v>
       </c>
-      <c r="C43">
-        <v>2</v>
-      </c>
-      <c r="D43">
+      <c r="C45">
         <v>340042</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>78</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>79</v>
       </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-      <c r="D44">
+      <c r="C46">
         <v>340043</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>80</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>0</v>
       </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45">
+      <c r="C47">
         <v>340044</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>81</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
         <v>82</v>
       </c>
-      <c r="C46">
-        <v>2</v>
-      </c>
-      <c r="D46">
+      <c r="C48">
         <v>340045</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+      <c r="E48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>81</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>82</v>
       </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47">
+      <c r="C49">
         <v>340046</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>83</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B50" t="s">
         <v>84</v>
       </c>
-      <c r="C48">
-        <v>2</v>
-      </c>
-      <c r="D48">
+      <c r="C50">
         <v>340047</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>85</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B51" t="s">
         <v>86</v>
       </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49">
+      <c r="C51">
         <v>340048</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>87</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B52" t="s">
         <v>88</v>
       </c>
-      <c r="C50">
-        <v>2</v>
-      </c>
-      <c r="D50">
+      <c r="C52">
         <v>340049</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>89</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B53" t="s">
         <v>90</v>
       </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="D51">
+      <c r="C53">
         <v>340050</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>91</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B54" t="s">
         <v>92</v>
       </c>
-      <c r="C52">
-        <v>2</v>
-      </c>
-      <c r="D52">
+      <c r="C54">
         <v>340051</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="E54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>91</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B55" t="s">
         <v>92</v>
       </c>
-      <c r="C53">
-        <v>2</v>
-      </c>
-      <c r="D53">
+      <c r="C55">
         <v>340052</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+      <c r="E55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>93</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B56" t="s">
         <v>94</v>
       </c>
-      <c r="C54">
-        <v>2</v>
-      </c>
-      <c r="D54">
+      <c r="C56">
         <v>340053</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="E56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>93</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B57" t="s">
         <v>94</v>
       </c>
-      <c r="C55">
-        <v>2</v>
-      </c>
-      <c r="D55">
+      <c r="C57">
         <v>340054</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+      <c r="E57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>95</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B58" t="s">
         <v>96</v>
       </c>
-      <c r="C56">
-        <v>2</v>
-      </c>
-      <c r="D56">
+      <c r="C58">
         <v>340055</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+      <c r="E58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>97</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B59" t="s">
         <v>98</v>
       </c>
-      <c r="C57">
-        <v>2</v>
-      </c>
-      <c r="D57">
+      <c r="C59">
         <v>340056</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="E59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>97</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B60" t="s">
         <v>98</v>
       </c>
-      <c r="C58">
-        <v>2</v>
-      </c>
-      <c r="D58">
+      <c r="C60">
         <v>340057</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+      <c r="E60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>99</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B61" t="s">
         <v>100</v>
       </c>
-      <c r="C59">
-        <v>2</v>
-      </c>
-      <c r="D59">
+      <c r="C61">
         <v>340058</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+      <c r="E61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>99</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B62" t="s">
         <v>100</v>
       </c>
-      <c r="C60">
-        <v>2</v>
-      </c>
-      <c r="D60">
+      <c r="C62">
         <v>340059</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="E62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>101</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B63" t="s">
         <v>102</v>
       </c>
-      <c r="C61">
-        <v>2</v>
-      </c>
-      <c r="D61">
+      <c r="C63">
         <v>340060</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+      <c r="E63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>101</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B64" t="s">
         <v>102</v>
       </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="D62">
+      <c r="C64">
         <v>340061</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+      <c r="E64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>103</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B65" t="s">
         <v>104</v>
       </c>
-      <c r="C63">
-        <v>2</v>
-      </c>
-      <c r="D63">
+      <c r="C65">
         <v>340062</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="E65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>103</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>104</v>
       </c>
-      <c r="C64">
-        <v>2</v>
-      </c>
-      <c r="D64">
+      <c r="C66">
         <v>340063</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+      <c r="E66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>105</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B67" t="s">
         <v>106</v>
       </c>
-      <c r="C65">
-        <v>2</v>
-      </c>
-      <c r="D65">
+      <c r="C67">
         <v>340064</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+      <c r="E67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>105</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B68" t="s">
         <v>106</v>
       </c>
-      <c r="C66">
-        <v>2</v>
-      </c>
-      <c r="D66">
+      <c r="C68">
         <v>340065</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="E68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>107</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B69" t="s">
         <v>108</v>
       </c>
-      <c r="C67">
-        <v>2</v>
-      </c>
-      <c r="D67">
+      <c r="C69">
         <v>340066</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="E69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>109</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B70" t="s">
         <v>110</v>
       </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
-      <c r="D68">
+      <c r="C70">
         <v>340067</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+      <c r="E70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>111</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B71" t="s">
         <v>112</v>
       </c>
-      <c r="C69">
-        <v>2</v>
-      </c>
-      <c r="D69">
+      <c r="C71">
         <v>340068</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="E71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>113</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B72" t="s">
         <v>114</v>
       </c>
-      <c r="C70">
-        <v>2</v>
-      </c>
-      <c r="D70">
+      <c r="C72">
         <v>340069</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+      <c r="E72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>115</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B73" t="s">
         <v>116</v>
       </c>
-      <c r="C71">
-        <v>2</v>
-      </c>
-      <c r="D71">
+      <c r="C73">
         <v>340070</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="E73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>117</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B74" t="s">
         <v>118</v>
       </c>
-      <c r="C72">
-        <v>2</v>
-      </c>
-      <c r="D72">
+      <c r="C74">
         <v>340071</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="E74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>119</v>
-      </c>
-      <c r="B73" t="s">
-        <v>120</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73">
-        <v>340072</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>121</v>
-      </c>
-      <c r="B74" t="s">
-        <v>122</v>
-      </c>
-      <c r="C74">
-        <v>2</v>
-      </c>
-      <c r="D74">
-        <v>340073</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>123</v>
       </c>
       <c r="B75" t="s">
         <v>120</v>
       </c>
       <c r="C75">
-        <v>2</v>
-      </c>
-      <c r="D75">
+        <v>340072</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>121</v>
+      </c>
+      <c r="B76" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76">
+        <v>340073</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" t="s">
+        <v>120</v>
+      </c>
+      <c r="C77">
         <v>340074</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+      <c r="E77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>124</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B78" t="s">
         <v>125</v>
       </c>
-      <c r="C76">
-        <v>2</v>
-      </c>
-      <c r="D76">
+      <c r="C78">
         <v>340075</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="E78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>126</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B79" t="s">
         <v>127</v>
       </c>
-      <c r="C77">
-        <v>2</v>
-      </c>
-      <c r="D77">
+      <c r="C79">
         <v>340076</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+      <c r="E79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>128</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B80" t="s">
         <v>129</v>
       </c>
-      <c r="C78">
-        <v>2</v>
-      </c>
-      <c r="D78">
+      <c r="C80">
         <v>340077</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="E80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>128</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B81" t="s">
         <v>129</v>
       </c>
-      <c r="C79">
-        <v>2</v>
-      </c>
-      <c r="D79">
+      <c r="C81">
         <v>340078</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+      <c r="E81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>130</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
         <v>131</v>
       </c>
-      <c r="C80">
-        <v>2</v>
-      </c>
-      <c r="D80">
+      <c r="C82">
         <v>340079</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="E82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>132</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B83" t="s">
         <v>133</v>
       </c>
-      <c r="C81">
-        <v>2</v>
-      </c>
-      <c r="D81">
+      <c r="C83">
         <v>340080</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="E83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>132</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B84" t="s">
         <v>133</v>
       </c>
-      <c r="C82">
-        <v>2</v>
-      </c>
-      <c r="D82">
+      <c r="C84">
         <v>340081</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="E84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>134</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B85" t="s">
         <v>135</v>
       </c>
-      <c r="C83">
-        <v>2</v>
-      </c>
-      <c r="D83">
+      <c r="C85">
         <v>340082</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="E85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>136</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B86" t="s">
         <v>137</v>
       </c>
-      <c r="C84">
-        <v>2</v>
-      </c>
-      <c r="D84">
+      <c r="C86">
         <v>340083</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="E86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>138</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B87" t="s">
         <v>56</v>
       </c>
-      <c r="C85">
-        <v>2</v>
-      </c>
-      <c r="D85">
+      <c r="C87">
         <v>340084</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="E87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>139</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B88" t="s">
         <v>140</v>
       </c>
-      <c r="C86">
-        <v>2</v>
-      </c>
-      <c r="D86">
+      <c r="C88">
         <v>340085</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="E88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>141</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>142</v>
       </c>
-      <c r="C87">
-        <v>2</v>
-      </c>
-      <c r="D87">
+      <c r="C89">
         <v>340086</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+      <c r="E89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>143</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B90" t="s">
         <v>45</v>
       </c>
-      <c r="C88">
-        <v>2</v>
-      </c>
-      <c r="D88">
+      <c r="C90">
         <v>340087</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="E90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>143</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B91" t="s">
         <v>45</v>
       </c>
-      <c r="C89">
-        <v>2</v>
-      </c>
-      <c r="D89">
+      <c r="C91">
         <v>340088</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="E91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>144</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B92" t="s">
         <v>145</v>
       </c>
-      <c r="C90">
-        <v>2</v>
-      </c>
-      <c r="D90">
+      <c r="C92">
         <v>340089</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="E92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>146</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B93" t="s">
         <v>147</v>
       </c>
-      <c r="C91">
-        <v>2</v>
-      </c>
-      <c r="D91">
+      <c r="C93">
         <v>340090</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+      <c r="E93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>148</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B94" t="s">
         <v>149</v>
       </c>
-      <c r="C92">
-        <v>2</v>
-      </c>
-      <c r="D92">
+      <c r="C94">
         <v>340091</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="E94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>150</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B95" t="s">
         <v>151</v>
       </c>
-      <c r="C93">
-        <v>2</v>
-      </c>
-      <c r="D93">
+      <c r="C95">
         <v>340092</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+      <c r="E95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>152</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B96" t="s">
         <v>153</v>
       </c>
-      <c r="C94">
-        <v>2</v>
-      </c>
-      <c r="D94">
+      <c r="C96">
         <v>340093</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+      <c r="E96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>154</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B97" t="s">
         <v>155</v>
       </c>
-      <c r="C95">
-        <v>2</v>
-      </c>
-      <c r="D95">
+      <c r="C97">
         <v>340094</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="E97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>156</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B98" t="s">
         <v>157</v>
       </c>
-      <c r="C96">
-        <v>2</v>
-      </c>
-      <c r="D96">
+      <c r="C98">
         <v>340095</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+      <c r="E98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>158</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B99" t="s">
         <v>159</v>
       </c>
-      <c r="C97">
-        <v>2</v>
-      </c>
-      <c r="D97">
+      <c r="C99">
         <v>340096</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+      <c r="E99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>160</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B100" t="s">
         <v>161</v>
       </c>
-      <c r="C98">
-        <v>2</v>
-      </c>
-      <c r="D98">
+      <c r="C100">
         <v>340097</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+      <c r="E100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>162</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B101" t="s">
         <v>163</v>
       </c>
-      <c r="C99">
-        <v>2</v>
-      </c>
-      <c r="D99">
+      <c r="C101">
         <v>340098</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+      <c r="E101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>164</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B102" t="s">
         <v>165</v>
       </c>
-      <c r="C100">
-        <v>2</v>
-      </c>
-      <c r="D100">
+      <c r="C102">
         <v>340099</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+      <c r="E102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>164</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B103" t="s">
         <v>165</v>
       </c>
-      <c r="C101">
-        <v>2</v>
-      </c>
-      <c r="D101">
+      <c r="C103">
         <v>340100</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+      <c r="E103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>166</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B104" t="s">
         <v>167</v>
       </c>
-      <c r="C102">
-        <v>2</v>
-      </c>
-      <c r="D102">
+      <c r="C104">
         <v>340101</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="E104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>168</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B105" t="s">
         <v>169</v>
       </c>
-      <c r="C103">
-        <v>2</v>
-      </c>
-      <c r="D103">
+      <c r="C105">
         <v>340102</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="E105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>170</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B106" t="s">
         <v>131</v>
       </c>
-      <c r="C104">
-        <v>2</v>
-      </c>
-      <c r="D104">
+      <c r="C106">
         <v>340103</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+      <c r="E106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>171</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B107" t="s">
         <v>172</v>
       </c>
-      <c r="C105">
-        <v>2</v>
-      </c>
-      <c r="D105">
+      <c r="C107">
         <v>340104</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="E107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>173</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B108" t="s">
         <v>174</v>
       </c>
-      <c r="C106">
-        <v>2</v>
-      </c>
-      <c r="D106">
+      <c r="C108">
         <v>340105</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+      <c r="E108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>175</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B109" t="s">
         <v>176</v>
       </c>
-      <c r="C107">
-        <v>2</v>
-      </c>
-      <c r="D107">
+      <c r="C109">
         <v>340106</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+      <c r="E109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>175</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B110" t="s">
         <v>176</v>
       </c>
-      <c r="C108">
-        <v>2</v>
-      </c>
-      <c r="D108">
+      <c r="C110">
         <v>340107</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+      <c r="E110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>177</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B111" t="s">
         <v>178</v>
       </c>
-      <c r="C109">
-        <v>2</v>
-      </c>
-      <c r="D109">
+      <c r="C111">
         <v>340108</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+      <c r="E111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>177</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B112" t="s">
         <v>178</v>
       </c>
-      <c r="C110">
-        <v>2</v>
-      </c>
-      <c r="D110">
+      <c r="C112">
         <v>340109</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+      <c r="E112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>179</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B113" t="s">
         <v>98</v>
       </c>
-      <c r="C111">
-        <v>2</v>
-      </c>
-      <c r="D111">
+      <c r="C113">
         <v>340110</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+      <c r="E113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>179</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B114" t="s">
         <v>98</v>
       </c>
-      <c r="C112">
-        <v>2</v>
-      </c>
-      <c r="D112">
+      <c r="C114">
         <v>340111</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+      <c r="E114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>180</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B115" t="s">
         <v>181</v>
       </c>
-      <c r="C113">
-        <v>2</v>
-      </c>
-      <c r="D113">
+      <c r="C115">
         <v>340112</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+      <c r="E115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>182</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B116" t="s">
         <v>183</v>
       </c>
-      <c r="C114">
-        <v>2</v>
-      </c>
-      <c r="D114">
+      <c r="C116">
         <v>340113</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+      <c r="E116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>184</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B117" t="s">
         <v>185</v>
       </c>
-      <c r="C115">
-        <v>2</v>
-      </c>
-      <c r="D115">
+      <c r="C117">
         <v>340114</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+      <c r="E117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>184</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B118" t="s">
         <v>185</v>
       </c>
-      <c r="C116">
-        <v>2</v>
-      </c>
-      <c r="D116">
+      <c r="C118">
         <v>340115</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+      <c r="E118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>186</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B119" t="s">
         <v>187</v>
       </c>
-      <c r="C117">
-        <v>2</v>
-      </c>
-      <c r="D117">
+      <c r="C119">
         <v>340116</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+      <c r="E119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>186</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B120" t="s">
         <v>187</v>
       </c>
-      <c r="C118">
-        <v>2</v>
-      </c>
-      <c r="D118">
+      <c r="C120">
         <v>340117</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+      <c r="E120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>188</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B121" t="s">
         <v>189</v>
       </c>
-      <c r="C119">
-        <v>2</v>
-      </c>
-      <c r="D119">
+      <c r="C121">
         <v>340118</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="E121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>188</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B122" t="s">
         <v>189</v>
       </c>
-      <c r="C120">
-        <v>2</v>
-      </c>
-      <c r="D120">
+      <c r="C122">
         <v>340119</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+      <c r="E122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>190</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B123" t="s">
         <v>11</v>
       </c>
-      <c r="C121">
-        <v>2</v>
-      </c>
-      <c r="D121">
+      <c r="C123">
         <v>340120</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+      <c r="E123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>191</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B124" t="s">
         <v>192</v>
       </c>
-      <c r="C122">
-        <v>2</v>
-      </c>
-      <c r="D122">
+      <c r="C124">
         <v>340121</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+      <c r="E124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>193</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B125" t="s">
         <v>114</v>
       </c>
-      <c r="C123">
-        <v>2</v>
-      </c>
-      <c r="D123">
+      <c r="C125">
         <v>340122</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+      <c r="E125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>194</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B126" t="s">
         <v>195</v>
       </c>
-      <c r="C124">
-        <v>2</v>
-      </c>
-      <c r="D124">
+      <c r="C126">
         <v>340123</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
+      <c r="E126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>196</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B127" t="s">
         <v>197</v>
       </c>
-      <c r="C125">
-        <v>2</v>
-      </c>
-      <c r="D125">
+      <c r="C127">
         <v>340124</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+      <c r="E127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>198</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B128" t="s">
         <v>199</v>
       </c>
-      <c r="C126">
-        <v>2</v>
-      </c>
-      <c r="D126">
+      <c r="C128">
         <v>340125</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+      <c r="E128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>200</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B129" t="s">
         <v>201</v>
       </c>
-      <c r="C127">
-        <v>2</v>
-      </c>
-      <c r="D127">
+      <c r="C129">
         <v>340126</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
+      <c r="E129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>202</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B130" t="s">
         <v>203</v>
       </c>
-      <c r="C128">
-        <v>2</v>
-      </c>
-      <c r="D128">
+      <c r="C130">
         <v>340127</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+      <c r="E130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>204</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B131" t="s">
         <v>205</v>
       </c>
-      <c r="C129">
-        <v>2</v>
-      </c>
-      <c r="D129">
+      <c r="C131">
         <v>340128</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
+      <c r="E131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>206</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B132" t="s">
         <v>207</v>
       </c>
-      <c r="C130">
-        <v>2</v>
-      </c>
-      <c r="D130">
+      <c r="C132">
         <v>340129</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+      <c r="E132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>208</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B133" t="s">
         <v>209</v>
       </c>
-      <c r="C131">
-        <v>2</v>
-      </c>
-      <c r="D131">
+      <c r="C133">
         <v>340130</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
+      <c r="E133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>210</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B134" t="s">
         <v>211</v>
       </c>
-      <c r="C132">
-        <v>2</v>
-      </c>
-      <c r="D132">
+      <c r="C134">
         <v>340131</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
+      <c r="E134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>212</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B135" t="s">
         <v>0</v>
       </c>
-      <c r="C133">
-        <v>2</v>
-      </c>
-      <c r="D133">
+      <c r="C135">
         <v>340132</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A134" t="s">
+      <c r="E135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>213</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B136" t="s">
         <v>214</v>
       </c>
-      <c r="C134">
-        <v>1</v>
-      </c>
-      <c r="D134">
+      <c r="C136">
         <v>34100</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A135" t="s">
+      <c r="E136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>215</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B137" t="s">
         <v>216</v>
       </c>
-      <c r="C135">
-        <v>1</v>
-      </c>
-      <c r="D135">
+      <c r="C137">
         <v>34101</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+      <c r="E137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>217</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B138" t="s">
         <v>218</v>
       </c>
-      <c r="C136">
-        <v>1</v>
-      </c>
-      <c r="D136">
+      <c r="C138">
         <v>34102</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
+      <c r="E138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>219</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B139" t="s">
         <v>220</v>
       </c>
-      <c r="C137">
-        <v>1</v>
-      </c>
-      <c r="D137">
+      <c r="C139">
         <v>34103</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
+      <c r="E139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>221</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B140" t="s">
         <v>222</v>
       </c>
-      <c r="C138">
-        <v>1</v>
-      </c>
-      <c r="D138">
+      <c r="C140">
         <v>34104</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
+      <c r="E140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>223</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B141" t="s">
         <v>224</v>
       </c>
-      <c r="C139">
-        <v>1</v>
-      </c>
-      <c r="D139">
+      <c r="C141">
         <v>34105</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
+      <c r="E141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>225</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B142" t="s">
         <v>226</v>
       </c>
-      <c r="C140">
-        <v>1</v>
-      </c>
-      <c r="D140">
+      <c r="C142">
         <v>34106</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
+      <c r="E142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>227</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B143" t="s">
         <v>228</v>
       </c>
-      <c r="C141">
-        <v>1</v>
-      </c>
-      <c r="D141">
+      <c r="C143">
         <v>34107</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
+      <c r="E143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>229</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B144" t="s">
         <v>230</v>
       </c>
-      <c r="C142">
-        <v>1</v>
-      </c>
-      <c r="D142">
+      <c r="C144">
         <v>34108</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
+      <c r="E144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>231</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B145" t="s">
         <v>232</v>
       </c>
-      <c r="C143">
-        <v>1</v>
-      </c>
-      <c r="D143">
+      <c r="C145">
         <v>34109</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
+      <c r="E145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>233</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B146" t="s">
         <v>234</v>
       </c>
-      <c r="C144">
-        <v>1</v>
-      </c>
-      <c r="D144">
+      <c r="C146">
         <v>34110</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+      <c r="E146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>235</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B147" t="s">
         <v>222</v>
       </c>
-      <c r="C145">
-        <v>1</v>
-      </c>
-      <c r="D145">
+      <c r="C147">
         <v>34111</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+      <c r="E147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>236</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B148" t="s">
         <v>322</v>
       </c>
-      <c r="C146">
-        <v>1</v>
-      </c>
-      <c r="D146">
+      <c r="C148">
         <v>34112</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+      <c r="E148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>237</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B149" t="s">
         <v>238</v>
       </c>
-      <c r="C147">
-        <v>1</v>
-      </c>
-      <c r="D147">
+      <c r="C149">
         <v>34113</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+      <c r="E149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>239</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B150" t="s">
         <v>240</v>
       </c>
-      <c r="C148">
-        <v>1</v>
-      </c>
-      <c r="D148">
+      <c r="C150">
         <v>34114</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
+      <c r="E150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>241</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B151" t="s">
         <v>242</v>
       </c>
-      <c r="C149">
-        <v>1</v>
-      </c>
-      <c r="D149">
+      <c r="C151">
         <v>34115</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
+      <c r="E151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>243</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B152" t="s">
         <v>244</v>
       </c>
-      <c r="C150">
-        <v>1</v>
-      </c>
-      <c r="D150">
+      <c r="C152">
         <v>34116</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
+      <c r="E152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>245</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B153" t="s">
         <v>246</v>
       </c>
-      <c r="C151">
-        <v>1</v>
-      </c>
-      <c r="D151">
+      <c r="C153">
         <v>34117</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
+      <c r="E153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>247</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B154" t="s">
         <v>248</v>
       </c>
-      <c r="C152">
-        <v>1</v>
-      </c>
-      <c r="D152">
+      <c r="C154">
         <v>34118</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A153" t="s">
+      <c r="E154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>249</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B155" t="s">
         <v>250</v>
       </c>
-      <c r="C153">
-        <v>1</v>
-      </c>
-      <c r="D153">
+      <c r="C155">
         <v>34119</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A154" t="s">
+      <c r="E155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>251</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B156" t="s">
         <v>252</v>
       </c>
-      <c r="C154">
-        <v>1</v>
-      </c>
-      <c r="D154">
+      <c r="C156">
         <v>34120</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
+      <c r="E156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>253</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B157" t="s">
         <v>254</v>
       </c>
-      <c r="C155">
-        <v>1</v>
-      </c>
-      <c r="D155">
+      <c r="C157">
         <v>34121</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
+      <c r="E157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>111</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B158" t="s">
         <v>255</v>
       </c>
-      <c r="C156">
-        <v>1</v>
-      </c>
-      <c r="D156">
+      <c r="C158">
         <v>34122</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A157" t="s">
+      <c r="E158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>256</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B159" t="s">
         <v>257</v>
       </c>
-      <c r="C157">
-        <v>1</v>
-      </c>
-      <c r="D157">
+      <c r="C159">
         <v>34123</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A158" t="s">
+      <c r="E159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>258</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B160" t="s">
         <v>131</v>
       </c>
-      <c r="C158">
-        <v>1</v>
-      </c>
-      <c r="D158">
+      <c r="C160">
         <v>34124</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A159" t="s">
+      <c r="E160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>259</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B161" t="s">
         <v>260</v>
       </c>
-      <c r="C159">
-        <v>1</v>
-      </c>
-      <c r="D159">
+      <c r="C161">
         <v>34125</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A160" t="s">
+      <c r="E161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>261</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B162" t="s">
         <v>262</v>
       </c>
-      <c r="C160">
-        <v>1</v>
-      </c>
-      <c r="D160">
+      <c r="C162">
         <v>34126</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+      <c r="E162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>263</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B163" t="s">
         <v>264</v>
       </c>
-      <c r="C161">
-        <v>1</v>
-      </c>
-      <c r="D161">
+      <c r="C163">
         <v>34127</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A162" t="s">
+      <c r="E163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>265</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B164" t="s">
         <v>266</v>
       </c>
-      <c r="C162">
-        <v>1</v>
-      </c>
-      <c r="D162">
+      <c r="C164">
         <v>34128</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
+      <c r="E164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>267</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B165" t="s">
         <v>268</v>
       </c>
-      <c r="C163">
-        <v>1</v>
-      </c>
-      <c r="D163">
+      <c r="C165">
         <v>34129</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A164" t="s">
+      <c r="E165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>269</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B166" t="s">
         <v>270</v>
       </c>
-      <c r="C164">
-        <v>1</v>
-      </c>
-      <c r="D164">
+      <c r="C166">
         <v>34130</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A165" t="s">
+      <c r="E166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>271</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B167" t="s">
         <v>45</v>
       </c>
-      <c r="C165">
-        <v>1</v>
-      </c>
-      <c r="D165">
+      <c r="C167">
         <v>34131</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A166" t="s">
+      <c r="E167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>272</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B168" t="s">
         <v>273</v>
       </c>
-      <c r="C166">
-        <v>1</v>
-      </c>
-      <c r="D166">
+      <c r="C168">
         <v>34132</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A167" t="s">
+      <c r="E168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>228</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B169" t="s">
         <v>274</v>
       </c>
-      <c r="C167">
-        <v>1</v>
-      </c>
-      <c r="D167">
+      <c r="C169">
         <v>34133</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A168" t="s">
+      <c r="E169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>275</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B170" t="s">
         <v>254</v>
       </c>
-      <c r="C168">
-        <v>1</v>
-      </c>
-      <c r="D168">
+      <c r="C170">
         <v>34134</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A169" t="s">
+      <c r="E170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>276</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B171" t="s">
         <v>277</v>
       </c>
-      <c r="C169">
-        <v>1</v>
-      </c>
-      <c r="D169">
+      <c r="C171">
         <v>34135</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A170" t="s">
+      <c r="E171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>278</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B172" t="s">
         <v>279</v>
       </c>
-      <c r="C170">
-        <v>1</v>
-      </c>
-      <c r="D170">
+      <c r="C172">
         <v>34136</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+      <c r="E172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>280</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B173" t="s">
         <v>281</v>
       </c>
-      <c r="C171">
-        <v>1</v>
-      </c>
-      <c r="D171">
+      <c r="C173">
         <v>34137</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A172" t="s">
+      <c r="E173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>282</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B174" t="s">
         <v>283</v>
       </c>
-      <c r="C172">
-        <v>1</v>
-      </c>
-      <c r="D172">
+      <c r="C174">
         <v>34138</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A173" t="s">
+      <c r="E174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>284</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B175" t="s">
         <v>285</v>
       </c>
-      <c r="C173">
-        <v>1</v>
-      </c>
-      <c r="D173">
+      <c r="C175">
         <v>34139</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A174" t="s">
+      <c r="E175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>286</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B176" t="s">
         <v>287</v>
       </c>
-      <c r="C174">
-        <v>1</v>
-      </c>
-      <c r="D174">
+      <c r="C176">
         <v>34140</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A175" t="s">
+      <c r="E176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>288</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B177" t="s">
         <v>176</v>
       </c>
-      <c r="C175">
-        <v>1</v>
-      </c>
-      <c r="D175">
+      <c r="C177">
         <v>34141</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A176" t="s">
+      <c r="E177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>289</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B178" t="s">
         <v>290</v>
       </c>
-      <c r="C176">
-        <v>1</v>
-      </c>
-      <c r="D176">
+      <c r="C178">
         <v>34142</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A177" t="s">
+      <c r="E178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>291</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B179" t="s">
         <v>292</v>
       </c>
-      <c r="C177">
-        <v>1</v>
-      </c>
-      <c r="D177">
+      <c r="C179">
         <v>34143</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A178" t="s">
+      <c r="E179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>293</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B180" t="s">
         <v>294</v>
       </c>
-      <c r="C178">
-        <v>1</v>
-      </c>
-      <c r="D178">
+      <c r="C180">
         <v>34144</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
+      <c r="E180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>295</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B181" t="s">
         <v>140</v>
       </c>
-      <c r="C179">
-        <v>1</v>
-      </c>
-      <c r="D179">
+      <c r="C181">
         <v>34145</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
+      <c r="E181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>296</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B182" t="s">
         <v>297</v>
       </c>
-      <c r="C180">
-        <v>1</v>
-      </c>
-      <c r="D180">
+      <c r="C182">
         <v>34146</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A181" t="s">
+      <c r="E182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>298</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B183" t="s">
         <v>299</v>
       </c>
-      <c r="C181">
-        <v>1</v>
-      </c>
-      <c r="D181">
+      <c r="C183">
         <v>34147</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A182" t="s">
+      <c r="E183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>326</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B184" t="s">
         <v>325</v>
       </c>
-      <c r="C182">
-        <v>1</v>
-      </c>
-      <c r="D182">
+      <c r="C184">
         <v>34148</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A183" t="s">
+      <c r="E184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>328</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B185" t="s">
         <v>327</v>
       </c>
-      <c r="C183">
-        <v>1</v>
-      </c>
-      <c r="D183">
+      <c r="C185">
         <v>34149</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A184" t="s">
+      <c r="E185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>329</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B186" t="s">
         <v>64</v>
       </c>
-      <c r="C184">
-        <v>1</v>
-      </c>
-      <c r="D184">
+      <c r="C186">
         <v>34150</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A185" t="s">
+      <c r="E186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>300</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B187" t="s">
         <v>301</v>
       </c>
-      <c r="C185">
-        <v>1</v>
-      </c>
-      <c r="D185">
+      <c r="C187">
         <v>34151</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A186" t="s">
+      <c r="E187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>302</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B188" t="s">
         <v>303</v>
       </c>
-      <c r="C186">
-        <v>1</v>
-      </c>
-      <c r="D186">
+      <c r="C188">
         <v>34152</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A187" t="s">
+      <c r="E188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>304</v>
       </c>
-      <c r="B187" t="s">
+      <c r="B189" t="s">
         <v>305</v>
       </c>
-      <c r="C187">
-        <v>1</v>
-      </c>
-      <c r="D187">
+      <c r="C189">
         <v>34153</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
+      <c r="E189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>306</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B190" t="s">
         <v>307</v>
       </c>
-      <c r="C188">
-        <v>1</v>
-      </c>
-      <c r="D188">
+      <c r="C190">
         <v>34154</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A189" t="s">
+      <c r="E190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>308</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B191" t="s">
         <v>309</v>
       </c>
-      <c r="C189">
-        <v>1</v>
-      </c>
-      <c r="D189">
+      <c r="C191">
         <v>34155</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A190" t="s">
+      <c r="E191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>324</v>
       </c>
-      <c r="B190" t="s">
+      <c r="B192" t="s">
         <v>323</v>
       </c>
-      <c r="C190">
-        <v>1</v>
-      </c>
-      <c r="D190">
+      <c r="C192">
         <v>34156</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A191" t="s">
+      <c r="E192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>310</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B193" t="s">
         <v>232</v>
       </c>
-      <c r="C191">
-        <v>1</v>
-      </c>
-      <c r="D191">
+      <c r="C193">
         <v>34157</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A192" t="s">
+      <c r="E193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>311</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B194" t="s">
         <v>312</v>
       </c>
-      <c r="C192">
-        <v>1</v>
-      </c>
-      <c r="D192">
+      <c r="C194">
         <v>34158</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A193" t="s">
+      <c r="E194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
         <v>313</v>
       </c>
-      <c r="B193" t="s">
+      <c r="B195" t="s">
         <v>314</v>
       </c>
-      <c r="C193">
-        <v>1</v>
-      </c>
-      <c r="D193">
+      <c r="C195">
         <v>34159</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A194" t="s">
+      <c r="E195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
         <v>315</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B196" t="s">
         <v>316</v>
       </c>
-      <c r="C194">
-        <v>1</v>
-      </c>
-      <c r="D194">
+      <c r="C196">
         <v>34160</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A195" t="s">
+      <c r="E196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
         <v>317</v>
       </c>
-      <c r="B195" t="s">
+      <c r="B197" t="s">
         <v>318</v>
       </c>
-      <c r="C195">
-        <v>1</v>
-      </c>
-      <c r="D195">
+      <c r="C197">
         <v>34161</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A196" t="s">
+      <c r="E197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>319</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B198" t="s">
         <v>319</v>
       </c>
-      <c r="C196">
-        <v>1</v>
-      </c>
-      <c r="D196">
+      <c r="C198">
         <v>404</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A197" t="s">
+      <c r="E198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>176</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B199" t="s">
         <v>222</v>
       </c>
-      <c r="C197">
-        <v>1</v>
-      </c>
-      <c r="D197">
+      <c r="C199">
         <v>34163</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A198" t="s">
+      <c r="E199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>320</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B200" t="s">
         <v>321</v>
       </c>
-      <c r="C198">
-        <v>1</v>
-      </c>
-      <c r="D198">
+      <c r="C200">
         <v>34164</v>
+      </c>
+      <c r="E200">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{B51DF5DD-3696-47D5-8BE6-65230F4978AD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>